<commit_message>
Updated the chronos template
</commit_message>
<xml_diff>
--- a/packages/frontend/public/chronos-templates/Chronos_Forecasting_Template.xlsx
+++ b/packages/frontend/public/chronos-templates/Chronos_Forecasting_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amariar/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7682AC89-A54B-2F4F-9F22-3310DD3075C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AE3B7E-C13A-6F47-AC19-BD47DA1FDD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29840" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
     </r>
   </si>
   <si>
-    <t>Please follow the instructions to the left, then save this template as a new excel sheet and upload it.</t>
+    <t>Please follow the instructions to the left, then save this template as a new excel sheet and upload</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,12 +197,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,7 +299,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -355,75 +349,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -976,9 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1381,22 +1305,6 @@
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0"/>
-  <conditionalFormatting sqref="B2:XFD33 B50:XFD1048576 D34:XFD49 B34:B49">
-    <cfRule type="containsBlanks" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(B2))=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>NOT(ISNUMBER(B2))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>ISNUMBER(B2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>ISNUMBER(A2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter>
@@ -1409,9 +1317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2092,69 +1998,10 @@
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0"/>
-  <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="containsBlanks" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>LEN(TRIM(A2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:XFD52 B55:XFD1048576 E53:XFD54 B53:C54">
-    <cfRule type="containsBlanks" priority="1" stopIfTrue="1">
-      <formula>LEN(TRIM(B2))=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>NOT(ISNUMBER(B2))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>ISNUMBER(B2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K000000Internal&amp;1#</oddHeader>
   </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="7" stopIfTrue="1" id="{AB26C187-5866-4C4A-843C-7594E1DD730C}">
-            <xm:f>y!$A2=""</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill patternType="solid">
-                  <bgColor theme="9" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-              <border>
-                <vertical/>
-                <horizontal/>
-              </border>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="8" operator="notEqual" id="{A0E94B81-C6EC-4772-A1BA-7879E5DCC8B9}">
-            <xm:f>y!$A2</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF0000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{FD01B0D8-B841-401C-9C98-2B0B96A134FF}">
-            <xm:f>y!$A2</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A2:A1048576</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update chronos forecasting template
</commit_message>
<xml_diff>
--- a/packages/frontend/public/chronos-templates/Chronos_Forecasting_Template.xlsx
+++ b/packages/frontend/public/chronos-templates/Chronos_Forecasting_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amariar/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\THOMAS_LOCAL\code\chronos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AE3B7E-C13A-6F47-AC19-BD47DA1FDD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE2B6BB-09CF-46CA-A7C7-A295BC6C6FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -632,24 +632,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="4.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
     <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
@@ -662,7 +662,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -673,7 +673,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
         <v>8</v>
       </c>
@@ -699,8 +699,8 @@
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
     </row>
-    <row r="5" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -710,7 +710,7 @@
       <c r="F6" s="8"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -718,57 +718,57 @@
       <c r="F7" s="11"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
@@ -777,105 +777,105 @@
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -892,26 +892,25 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K000000Internal&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="5"/>
+    <col min="3" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -919,7 +918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>42795</v>
       </c>
@@ -927,7 +926,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>42826</v>
       </c>
@@ -935,7 +934,7 @@
         <v>8350</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>42856</v>
       </c>
@@ -943,7 +942,7 @@
         <v>8570</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>42887</v>
       </c>
@@ -951,7 +950,7 @@
         <v>7700</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>42917</v>
       </c>
@@ -959,7 +958,7 @@
         <v>7080</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>42948</v>
       </c>
@@ -967,7 +966,7 @@
         <v>6520</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>42979</v>
       </c>
@@ -975,7 +974,7 @@
         <v>6070</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43009</v>
       </c>
@@ -983,7 +982,7 @@
         <v>6650</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43040</v>
       </c>
@@ -991,7 +990,7 @@
         <v>6830</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43070</v>
       </c>
@@ -999,7 +998,7 @@
         <v>5710</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43101</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>5260</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43132</v>
       </c>
@@ -1015,7 +1014,7 @@
         <v>5470</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43160</v>
       </c>
@@ -1023,7 +1022,7 @@
         <v>7870</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43191</v>
       </c>
@@ -1031,7 +1030,7 @@
         <v>7360</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43221</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>8470</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43252</v>
       </c>
@@ -1047,7 +1046,7 @@
         <v>7880</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43282</v>
       </c>
@@ -1055,7 +1054,7 @@
         <v>6750</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43313</v>
       </c>
@@ -1063,7 +1062,7 @@
         <v>6860</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43344</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>6220</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43374</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>6650</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43405</v>
       </c>
@@ -1087,7 +1086,7 @@
         <v>5450</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43435</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43466</v>
       </c>
@@ -1103,7 +1102,7 @@
         <v>4970</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43497</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>5550</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43525</v>
       </c>
@@ -1119,7 +1118,7 @@
         <v>7750</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43556</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>7760</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>43586</v>
       </c>
@@ -1135,7 +1134,7 @@
         <v>7190</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43617</v>
       </c>
@@ -1143,7 +1142,7 @@
         <v>7440</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43647</v>
       </c>
@@ -1151,7 +1150,7 @@
         <v>6590</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43678</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>6210</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43709</v>
       </c>
@@ -1167,7 +1166,7 @@
         <v>6010</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43739</v>
       </c>
@@ -1175,7 +1174,7 @@
         <v>6390</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43770</v>
       </c>
@@ -1183,7 +1182,7 @@
         <v>5343</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43800</v>
       </c>
@@ -1191,7 +1190,7 @@
         <v>6978</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43831</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>6201</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43862</v>
       </c>
@@ -1207,7 +1206,7 @@
         <v>7923</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43891</v>
       </c>
@@ -1215,7 +1214,7 @@
         <v>7673</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43922</v>
       </c>
@@ -1223,7 +1222,7 @@
         <v>7897</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43952</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>8107</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43983</v>
       </c>
@@ -1239,7 +1238,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>44013</v>
       </c>
@@ -1247,7 +1246,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>44044</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>6666</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>44075</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>8083</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44105</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44136</v>
       </c>
@@ -1279,7 +1278,7 @@
         <v>5415</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>44166</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>5775</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>44197</v>
       </c>
@@ -1295,37 +1294,132 @@
         <v>6752</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>44228</v>
       </c>
       <c r="B49" s="5">
         <v>7544</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>44256</v>
+      </c>
+      <c r="B50" s="5">
+        <v>7001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>44287</v>
+      </c>
+      <c r="B51" s="5">
+        <v>7332</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
+        <v>44317</v>
+      </c>
+      <c r="B52" s="5">
+        <v>8201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>44348</v>
+      </c>
+      <c r="B53" s="5">
+        <v>6932</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>44378</v>
+      </c>
+      <c r="B54" s="5">
+        <v>5988</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="4">
+        <v>44409</v>
+      </c>
+      <c r="B55" s="5">
+        <v>6450</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
+        <v>44440</v>
+      </c>
+      <c r="B56" s="5">
+        <v>7923</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="4">
+        <v>44470</v>
+      </c>
+      <c r="B57" s="5">
+        <v>6021</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="4">
+        <v>44501</v>
+      </c>
+      <c r="B58" s="5">
+        <v>5302</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="4">
+        <v>44531</v>
+      </c>
+      <c r="B59" s="5">
+        <v>5542</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="4">
+        <v>44562</v>
+      </c>
+      <c r="B60" s="5">
+        <v>6450</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="4">
+        <v>44593</v>
+      </c>
+      <c r="B61" s="5">
+        <v>7203</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K000000Internal&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="5"/>
+    <col min="1" max="1" width="12.44140625" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1336,7 +1430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>42795</v>
       </c>
@@ -1347,7 +1441,7 @@
         <v>7264</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>42826</v>
       </c>
@@ -1358,7 +1452,7 @@
         <v>7215</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>42856</v>
       </c>
@@ -1369,7 +1463,7 @@
         <v>7022</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>42887</v>
       </c>
@@ -1380,7 +1474,7 @@
         <v>7040</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>42917</v>
       </c>
@@ -1391,7 +1485,7 @@
         <v>6966</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>42948</v>
       </c>
@@ -1402,7 +1496,7 @@
         <v>6984</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>42979</v>
       </c>
@@ -1413,7 +1507,7 @@
         <v>7025</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43009</v>
       </c>
@@ -1424,7 +1518,7 @@
         <v>7082</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43040</v>
       </c>
@@ -1435,7 +1529,7 @@
         <v>6956</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43070</v>
       </c>
@@ -1446,7 +1540,7 @@
         <v>7014</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43101</v>
       </c>
@@ -1457,7 +1551,7 @@
         <v>7067</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43132</v>
       </c>
@@ -1468,7 +1562,7 @@
         <v>7099</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43160</v>
       </c>
@@ -1479,7 +1573,7 @@
         <v>7046</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43191</v>
       </c>
@@ -1490,7 +1584,7 @@
         <v>7139</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43221</v>
       </c>
@@ -1501,7 +1595,7 @@
         <v>7011</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43252</v>
       </c>
@@ -1512,7 +1606,7 @@
         <v>7022</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43282</v>
       </c>
@@ -1523,7 +1617,7 @@
         <v>7084</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43313</v>
       </c>
@@ -1534,7 +1628,7 @@
         <v>7036</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43344</v>
       </c>
@@ -1545,7 +1639,7 @@
         <v>7098</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43374</v>
       </c>
@@ -1556,7 +1650,7 @@
         <v>7083</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43405</v>
       </c>
@@ -1567,7 +1661,7 @@
         <v>7045</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43435</v>
       </c>
@@ -1578,7 +1672,7 @@
         <v>7057</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43466</v>
       </c>
@@ -1589,7 +1683,7 @@
         <v>6986</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43497</v>
       </c>
@@ -1600,7 +1694,7 @@
         <v>6937</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43525</v>
       </c>
@@ -1611,7 +1705,7 @@
         <v>6927</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43556</v>
       </c>
@@ -1622,7 +1716,7 @@
         <v>6953</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>43586</v>
       </c>
@@ -1633,7 +1727,7 @@
         <v>7007</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43617</v>
       </c>
@@ -1644,7 +1738,7 @@
         <v>6949</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43647</v>
       </c>
@@ -1655,7 +1749,7 @@
         <v>6930</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43678</v>
       </c>
@@ -1666,7 +1760,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43709</v>
       </c>
@@ -1677,7 +1771,7 @@
         <v>6956</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43739</v>
       </c>
@@ -1688,7 +1782,7 @@
         <v>6946</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43770</v>
       </c>
@@ -1699,7 +1793,7 @@
         <v>6866</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43800</v>
       </c>
@@ -1710,7 +1804,7 @@
         <v>6814</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43831</v>
       </c>
@@ -1721,7 +1815,7 @@
         <v>6806</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43862</v>
       </c>
@@ -1732,7 +1826,7 @@
         <v>6990</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43891</v>
       </c>
@@ -1743,7 +1837,7 @@
         <v>6897</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43922</v>
       </c>
@@ -1754,7 +1848,7 @@
         <v>6985</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43952</v>
       </c>
@@ -1765,7 +1859,7 @@
         <v>6911</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43983</v>
       </c>
@@ -1776,7 +1870,7 @@
         <v>6842</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>44013</v>
       </c>
@@ -1787,7 +1881,7 @@
         <v>6873</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>44044</v>
       </c>
@@ -1798,7 +1892,7 @@
         <v>6986</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>44075</v>
       </c>
@@ -1809,7 +1903,7 @@
         <v>6998</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44105</v>
       </c>
@@ -1820,7 +1914,7 @@
         <v>6976</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44136</v>
       </c>
@@ -1831,7 +1925,7 @@
         <v>6952</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>44166</v>
       </c>
@@ -1842,7 +1936,7 @@
         <v>6805</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>44197</v>
       </c>
@@ -1853,7 +1947,7 @@
         <v>6889</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>44228</v>
       </c>
@@ -1864,7 +1958,7 @@
         <v>6969</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>44256</v>
       </c>
@@ -1875,7 +1969,7 @@
         <v>6887</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>44287</v>
       </c>
@@ -1886,7 +1980,7 @@
         <v>6878</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>44317</v>
       </c>
@@ -1897,7 +1991,7 @@
         <v>6979</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>44348</v>
       </c>
@@ -1908,7 +2002,7 @@
         <v>6962</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>44378</v>
       </c>
@@ -1919,7 +2013,7 @@
         <v>6862</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>44409</v>
       </c>
@@ -1930,7 +2024,7 @@
         <v>6905</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>44440</v>
       </c>
@@ -1941,7 +2035,7 @@
         <v>6861</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>44470</v>
       </c>
@@ -1952,7 +2046,7 @@
         <v>6801</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>44501</v>
       </c>
@@ -1963,7 +2057,7 @@
         <v>6889</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>44531</v>
       </c>
@@ -1974,7 +2068,7 @@
         <v>6865</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>44562</v>
       </c>
@@ -1985,7 +2079,7 @@
         <v>6966</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>44593</v>
       </c>
@@ -1994,14 +2088,143 @@
       </c>
       <c r="C61" s="5">
         <v>6954</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="4">
+        <v>44621</v>
+      </c>
+      <c r="B62" s="5">
+        <v>3000</v>
+      </c>
+      <c r="C62" s="5">
+        <v>6893</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="4">
+        <v>44652</v>
+      </c>
+      <c r="B63" s="5">
+        <v>3121</v>
+      </c>
+      <c r="C63" s="5">
+        <v>6751</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="4">
+        <v>44682</v>
+      </c>
+      <c r="B64" s="5">
+        <v>3240</v>
+      </c>
+      <c r="C64" s="5">
+        <v>6678</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="4">
+        <v>44713</v>
+      </c>
+      <c r="B65" s="5">
+        <v>2425</v>
+      </c>
+      <c r="C65" s="5">
+        <v>6816</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="4">
+        <v>44743</v>
+      </c>
+      <c r="B66" s="5">
+        <v>2555</v>
+      </c>
+      <c r="C66" s="5">
+        <v>6724</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="4">
+        <v>44774</v>
+      </c>
+      <c r="B67" s="5">
+        <v>2345</v>
+      </c>
+      <c r="C67" s="5">
+        <v>6677</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="4">
+        <v>44805</v>
+      </c>
+      <c r="B68" s="5">
+        <v>2745</v>
+      </c>
+      <c r="C68" s="5">
+        <v>6344</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="4">
+        <v>44835</v>
+      </c>
+      <c r="B69" s="5">
+        <v>2464</v>
+      </c>
+      <c r="C69" s="5">
+        <v>6433</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="4">
+        <v>44866</v>
+      </c>
+      <c r="B70" s="5">
+        <v>2334</v>
+      </c>
+      <c r="C70" s="5">
+        <v>6441</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="4">
+        <v>44896</v>
+      </c>
+      <c r="B71" s="5">
+        <v>2131</v>
+      </c>
+      <c r="C71" s="5">
+        <v>6454</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="4">
+        <v>44927</v>
+      </c>
+      <c r="B72" s="5">
+        <v>1998</v>
+      </c>
+      <c r="C72" s="5">
+        <v>6321</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
+        <v>44958</v>
+      </c>
+      <c r="B73" s="5">
+        <v>2034</v>
+      </c>
+      <c r="C73" s="5">
+        <v>6212</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K000000Internal&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update chronos forecasting template (#2290)
</commit_message>
<xml_diff>
--- a/packages/frontend/public/chronos-templates/Chronos_Forecasting_Template.xlsx
+++ b/packages/frontend/public/chronos-templates/Chronos_Forecasting_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amariar/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\THOMAS_LOCAL\code\chronos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AE3B7E-C13A-6F47-AC19-BD47DA1FDD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE2B6BB-09CF-46CA-A7C7-A295BC6C6FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -632,24 +632,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="4.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
     <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
@@ -662,7 +662,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -673,7 +673,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
         <v>8</v>
       </c>
@@ -699,8 +699,8 @@
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
     </row>
-    <row r="5" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -710,7 +710,7 @@
       <c r="F6" s="8"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -718,57 +718,57 @@
       <c r="F7" s="11"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
@@ -777,105 +777,105 @@
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -892,26 +892,25 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K000000Internal&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="5"/>
+    <col min="3" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -919,7 +918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>42795</v>
       </c>
@@ -927,7 +926,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>42826</v>
       </c>
@@ -935,7 +934,7 @@
         <v>8350</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>42856</v>
       </c>
@@ -943,7 +942,7 @@
         <v>8570</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>42887</v>
       </c>
@@ -951,7 +950,7 @@
         <v>7700</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>42917</v>
       </c>
@@ -959,7 +958,7 @@
         <v>7080</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>42948</v>
       </c>
@@ -967,7 +966,7 @@
         <v>6520</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>42979</v>
       </c>
@@ -975,7 +974,7 @@
         <v>6070</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43009</v>
       </c>
@@ -983,7 +982,7 @@
         <v>6650</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43040</v>
       </c>
@@ -991,7 +990,7 @@
         <v>6830</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43070</v>
       </c>
@@ -999,7 +998,7 @@
         <v>5710</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43101</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>5260</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43132</v>
       </c>
@@ -1015,7 +1014,7 @@
         <v>5470</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43160</v>
       </c>
@@ -1023,7 +1022,7 @@
         <v>7870</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43191</v>
       </c>
@@ -1031,7 +1030,7 @@
         <v>7360</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43221</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>8470</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43252</v>
       </c>
@@ -1047,7 +1046,7 @@
         <v>7880</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43282</v>
       </c>
@@ -1055,7 +1054,7 @@
         <v>6750</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43313</v>
       </c>
@@ -1063,7 +1062,7 @@
         <v>6860</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43344</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>6220</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43374</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>6650</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43405</v>
       </c>
@@ -1087,7 +1086,7 @@
         <v>5450</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43435</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43466</v>
       </c>
@@ -1103,7 +1102,7 @@
         <v>4970</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43497</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>5550</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43525</v>
       </c>
@@ -1119,7 +1118,7 @@
         <v>7750</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43556</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>7760</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>43586</v>
       </c>
@@ -1135,7 +1134,7 @@
         <v>7190</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43617</v>
       </c>
@@ -1143,7 +1142,7 @@
         <v>7440</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43647</v>
       </c>
@@ -1151,7 +1150,7 @@
         <v>6590</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43678</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>6210</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43709</v>
       </c>
@@ -1167,7 +1166,7 @@
         <v>6010</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43739</v>
       </c>
@@ -1175,7 +1174,7 @@
         <v>6390</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43770</v>
       </c>
@@ -1183,7 +1182,7 @@
         <v>5343</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43800</v>
       </c>
@@ -1191,7 +1190,7 @@
         <v>6978</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43831</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>6201</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43862</v>
       </c>
@@ -1207,7 +1206,7 @@
         <v>7923</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43891</v>
       </c>
@@ -1215,7 +1214,7 @@
         <v>7673</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43922</v>
       </c>
@@ -1223,7 +1222,7 @@
         <v>7897</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43952</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>8107</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43983</v>
       </c>
@@ -1239,7 +1238,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>44013</v>
       </c>
@@ -1247,7 +1246,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>44044</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>6666</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>44075</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>8083</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44105</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44136</v>
       </c>
@@ -1279,7 +1278,7 @@
         <v>5415</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>44166</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>5775</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>44197</v>
       </c>
@@ -1295,37 +1294,132 @@
         <v>6752</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>44228</v>
       </c>
       <c r="B49" s="5">
         <v>7544</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>44256</v>
+      </c>
+      <c r="B50" s="5">
+        <v>7001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>44287</v>
+      </c>
+      <c r="B51" s="5">
+        <v>7332</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
+        <v>44317</v>
+      </c>
+      <c r="B52" s="5">
+        <v>8201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>44348</v>
+      </c>
+      <c r="B53" s="5">
+        <v>6932</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>44378</v>
+      </c>
+      <c r="B54" s="5">
+        <v>5988</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="4">
+        <v>44409</v>
+      </c>
+      <c r="B55" s="5">
+        <v>6450</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
+        <v>44440</v>
+      </c>
+      <c r="B56" s="5">
+        <v>7923</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="4">
+        <v>44470</v>
+      </c>
+      <c r="B57" s="5">
+        <v>6021</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="4">
+        <v>44501</v>
+      </c>
+      <c r="B58" s="5">
+        <v>5302</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="4">
+        <v>44531</v>
+      </c>
+      <c r="B59" s="5">
+        <v>5542</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="4">
+        <v>44562</v>
+      </c>
+      <c r="B60" s="5">
+        <v>6450</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="4">
+        <v>44593</v>
+      </c>
+      <c r="B61" s="5">
+        <v>7203</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K000000Internal&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="5"/>
+    <col min="1" max="1" width="12.44140625" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1336,7 +1430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>42795</v>
       </c>
@@ -1347,7 +1441,7 @@
         <v>7264</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>42826</v>
       </c>
@@ -1358,7 +1452,7 @@
         <v>7215</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>42856</v>
       </c>
@@ -1369,7 +1463,7 @@
         <v>7022</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>42887</v>
       </c>
@@ -1380,7 +1474,7 @@
         <v>7040</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>42917</v>
       </c>
@@ -1391,7 +1485,7 @@
         <v>6966</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>42948</v>
       </c>
@@ -1402,7 +1496,7 @@
         <v>6984</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>42979</v>
       </c>
@@ -1413,7 +1507,7 @@
         <v>7025</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43009</v>
       </c>
@@ -1424,7 +1518,7 @@
         <v>7082</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43040</v>
       </c>
@@ -1435,7 +1529,7 @@
         <v>6956</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43070</v>
       </c>
@@ -1446,7 +1540,7 @@
         <v>7014</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43101</v>
       </c>
@@ -1457,7 +1551,7 @@
         <v>7067</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43132</v>
       </c>
@@ -1468,7 +1562,7 @@
         <v>7099</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43160</v>
       </c>
@@ -1479,7 +1573,7 @@
         <v>7046</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43191</v>
       </c>
@@ -1490,7 +1584,7 @@
         <v>7139</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43221</v>
       </c>
@@ -1501,7 +1595,7 @@
         <v>7011</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43252</v>
       </c>
@@ -1512,7 +1606,7 @@
         <v>7022</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43282</v>
       </c>
@@ -1523,7 +1617,7 @@
         <v>7084</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43313</v>
       </c>
@@ -1534,7 +1628,7 @@
         <v>7036</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43344</v>
       </c>
@@ -1545,7 +1639,7 @@
         <v>7098</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43374</v>
       </c>
@@ -1556,7 +1650,7 @@
         <v>7083</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43405</v>
       </c>
@@ -1567,7 +1661,7 @@
         <v>7045</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43435</v>
       </c>
@@ -1578,7 +1672,7 @@
         <v>7057</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43466</v>
       </c>
@@ -1589,7 +1683,7 @@
         <v>6986</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43497</v>
       </c>
@@ -1600,7 +1694,7 @@
         <v>6937</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43525</v>
       </c>
@@ -1611,7 +1705,7 @@
         <v>6927</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43556</v>
       </c>
@@ -1622,7 +1716,7 @@
         <v>6953</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>43586</v>
       </c>
@@ -1633,7 +1727,7 @@
         <v>7007</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43617</v>
       </c>
@@ -1644,7 +1738,7 @@
         <v>6949</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43647</v>
       </c>
@@ -1655,7 +1749,7 @@
         <v>6930</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43678</v>
       </c>
@@ -1666,7 +1760,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43709</v>
       </c>
@@ -1677,7 +1771,7 @@
         <v>6956</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43739</v>
       </c>
@@ -1688,7 +1782,7 @@
         <v>6946</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43770</v>
       </c>
@@ -1699,7 +1793,7 @@
         <v>6866</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43800</v>
       </c>
@@ -1710,7 +1804,7 @@
         <v>6814</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43831</v>
       </c>
@@ -1721,7 +1815,7 @@
         <v>6806</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43862</v>
       </c>
@@ -1732,7 +1826,7 @@
         <v>6990</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43891</v>
       </c>
@@ -1743,7 +1837,7 @@
         <v>6897</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43922</v>
       </c>
@@ -1754,7 +1848,7 @@
         <v>6985</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43952</v>
       </c>
@@ -1765,7 +1859,7 @@
         <v>6911</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43983</v>
       </c>
@@ -1776,7 +1870,7 @@
         <v>6842</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>44013</v>
       </c>
@@ -1787,7 +1881,7 @@
         <v>6873</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>44044</v>
       </c>
@@ -1798,7 +1892,7 @@
         <v>6986</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>44075</v>
       </c>
@@ -1809,7 +1903,7 @@
         <v>6998</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44105</v>
       </c>
@@ -1820,7 +1914,7 @@
         <v>6976</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44136</v>
       </c>
@@ -1831,7 +1925,7 @@
         <v>6952</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>44166</v>
       </c>
@@ -1842,7 +1936,7 @@
         <v>6805</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>44197</v>
       </c>
@@ -1853,7 +1947,7 @@
         <v>6889</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>44228</v>
       </c>
@@ -1864,7 +1958,7 @@
         <v>6969</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>44256</v>
       </c>
@@ -1875,7 +1969,7 @@
         <v>6887</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>44287</v>
       </c>
@@ -1886,7 +1980,7 @@
         <v>6878</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>44317</v>
       </c>
@@ -1897,7 +1991,7 @@
         <v>6979</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>44348</v>
       </c>
@@ -1908,7 +2002,7 @@
         <v>6962</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>44378</v>
       </c>
@@ -1919,7 +2013,7 @@
         <v>6862</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>44409</v>
       </c>
@@ -1930,7 +2024,7 @@
         <v>6905</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>44440</v>
       </c>
@@ -1941,7 +2035,7 @@
         <v>6861</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>44470</v>
       </c>
@@ -1952,7 +2046,7 @@
         <v>6801</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>44501</v>
       </c>
@@ -1963,7 +2057,7 @@
         <v>6889</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>44531</v>
       </c>
@@ -1974,7 +2068,7 @@
         <v>6865</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>44562</v>
       </c>
@@ -1985,7 +2079,7 @@
         <v>6966</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>44593</v>
       </c>
@@ -1994,14 +2088,143 @@
       </c>
       <c r="C61" s="5">
         <v>6954</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="4">
+        <v>44621</v>
+      </c>
+      <c r="B62" s="5">
+        <v>3000</v>
+      </c>
+      <c r="C62" s="5">
+        <v>6893</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="4">
+        <v>44652</v>
+      </c>
+      <c r="B63" s="5">
+        <v>3121</v>
+      </c>
+      <c r="C63" s="5">
+        <v>6751</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="4">
+        <v>44682</v>
+      </c>
+      <c r="B64" s="5">
+        <v>3240</v>
+      </c>
+      <c r="C64" s="5">
+        <v>6678</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="4">
+        <v>44713</v>
+      </c>
+      <c r="B65" s="5">
+        <v>2425</v>
+      </c>
+      <c r="C65" s="5">
+        <v>6816</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="4">
+        <v>44743</v>
+      </c>
+      <c r="B66" s="5">
+        <v>2555</v>
+      </c>
+      <c r="C66" s="5">
+        <v>6724</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="4">
+        <v>44774</v>
+      </c>
+      <c r="B67" s="5">
+        <v>2345</v>
+      </c>
+      <c r="C67" s="5">
+        <v>6677</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="4">
+        <v>44805</v>
+      </c>
+      <c r="B68" s="5">
+        <v>2745</v>
+      </c>
+      <c r="C68" s="5">
+        <v>6344</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="4">
+        <v>44835</v>
+      </c>
+      <c r="B69" s="5">
+        <v>2464</v>
+      </c>
+      <c r="C69" s="5">
+        <v>6433</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="4">
+        <v>44866</v>
+      </c>
+      <c r="B70" s="5">
+        <v>2334</v>
+      </c>
+      <c r="C70" s="5">
+        <v>6441</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="4">
+        <v>44896</v>
+      </c>
+      <c r="B71" s="5">
+        <v>2131</v>
+      </c>
+      <c r="C71" s="5">
+        <v>6454</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="4">
+        <v>44927</v>
+      </c>
+      <c r="B72" s="5">
+        <v>1998</v>
+      </c>
+      <c r="C72" s="5">
+        <v>6321</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
+        <v>44958</v>
+      </c>
+      <c r="B73" s="5">
+        <v>2034</v>
+      </c>
+      <c r="C73" s="5">
+        <v>6212</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K000000Internal&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>